<commit_message>
feat: correções do modelo da tela
</commit_message>
<xml_diff>
--- a/assets/toy_problem_copy_2.xlsx
+++ b/assets/toy_problem_copy_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-projetos\fundaIA\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87457147-C672-43F7-ABC9-B37F0316FBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706335D3-E900-4A44-B5CB-ABD136FC141F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Elemento</t>
   </si>
@@ -85,25 +85,16 @@
   </si>
   <si>
     <t>P05</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>4.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +106,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -164,10 +162,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,12 +189,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,7 +460,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F2" sqref="F2:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,49 +519,49 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="9">
         <v>0.25</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="9">
         <v>1.2</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>43</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9">
         <v>377.3</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="9">
         <v>-1.9</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="9">
         <v>259.2</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="9">
         <v>-27.8</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="9">
         <v>0.1</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="9">
         <v>383.8</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="9">
         <v>27.7</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="9">
         <v>0.2</v>
       </c>
     </row>
@@ -566,49 +569,49 @@
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>0.3</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="9">
         <v>1.5</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>35</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="7">
+      <c r="F3" s="8">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8">
+        <v>8</v>
+      </c>
+      <c r="H3" s="9">
         <v>855.5</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="9">
         <v>-3.7</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="9">
         <v>9.1999999999999993</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="9">
         <v>891.9</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="9">
         <v>-60</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="9">
         <v>0.6</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="9">
         <v>908.5</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="9">
         <v>-36.9</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="9">
         <v>0.4</v>
       </c>
     </row>
@@ -616,49 +619,49 @@
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>0.25</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="9">
         <v>1.2</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>45</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="F4" s="8">
+        <v>4</v>
+      </c>
+      <c r="G4" s="8">
+        <v>4</v>
+      </c>
+      <c r="H4" s="9">
         <v>478.6</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="9">
         <v>-3.1</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="9">
         <v>5</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="9">
         <v>496</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="9">
         <v>-27.6</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="9">
         <v>0.7</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="9">
         <v>508</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="9">
         <v>-27.6</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="9">
         <v>0.7</v>
       </c>
     </row>

</xml_diff>